<commit_message>
[PHOENIX-5999] Modified sewerage tax module
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/SewerageTaxTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/SewerageTaxTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -28,7 +28,10 @@
     <t xml:space="preserve">propertyType</t>
   </si>
   <si>
-    <t xml:space="preserve">noOfClosets</t>
+    <t xml:space="preserve">noOfClosetsResidential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noOfClosetsNonResidential</t>
   </si>
   <si>
     <t xml:space="preserve">documentNumber</t>
@@ -40,6 +43,9 @@
     <t xml:space="preserve">RESIDENTIAL</t>
   </si>
   <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
     <t xml:space="preserve">change1</t>
   </si>
   <si>
@@ -50,14 +56,24 @@
   </si>
   <si>
     <t xml:space="preserve">change2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creation3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIXED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -130,12 +146,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -156,19 +176,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -184,60 +205,109 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>123</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>5</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>456</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="E5" s="0" t="n">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>456</v>
       </c>
     </row>

</xml_diff>